<commit_message>
Entscheidungmatrix | First Example Values
Changes in the README.TXT to keep it at the current State
I filled the First Values in the "Entscheidungsmatrix" but they still need to be checkt
</commit_message>
<xml_diff>
--- a/Entscheidungsmatrix.xlsx
+++ b/Entscheidungsmatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F273CDC-4EC8-4A26-A130-8244D23CBDD2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C2D091D-88ED-4BE6-8182-8E41D6EB7078}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -294,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -329,6 +329,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -612,7 +613,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,22 +692,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="C4" s="11">
+        <v>6</v>
+      </c>
       <c r="D4" s="12">
         <f>C4*(B4/100)</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="12"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="E4" s="12">
+        <v>2</v>
+      </c>
       <c r="F4" s="15">
         <f>E4*($B4/100)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="12"/>
+        <v>0.1</v>
+      </c>
+      <c r="G4" s="12">
+        <v>7</v>
+      </c>
       <c r="H4" s="15">
         <f>G4*($B4/100)</f>
-        <v>0</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="15">
@@ -719,22 +726,26 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="14">
         <f t="shared" ref="D5:D11" si="0">C5*(B5/100)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="14">
+        <v>7</v>
+      </c>
       <c r="F5" s="15">
         <f>E5*($B5/100)</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="14"/>
+        <v>2.1</v>
+      </c>
+      <c r="G5" s="14">
+        <v>7</v>
+      </c>
       <c r="H5" s="15">
         <f>G5*($B5/100)</f>
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="15">
@@ -747,22 +758,28 @@
         <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="C6" s="13">
+        <v>9</v>
+      </c>
       <c r="D6" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="14"/>
+        <v>0.9</v>
+      </c>
+      <c r="E6" s="14">
+        <v>9</v>
+      </c>
       <c r="F6" s="15">
         <f t="shared" ref="F6:H11" si="1">E6*($B6/100)</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="14"/>
+        <v>0.9</v>
+      </c>
+      <c r="G6" s="22">
+        <v>9</v>
+      </c>
       <c r="H6" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="15">
@@ -775,22 +792,28 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="C7" s="13">
+        <v>9</v>
+      </c>
       <c r="D7" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="14"/>
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="22">
+        <v>9</v>
+      </c>
       <c r="F7" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="14"/>
+        <v>0.9</v>
+      </c>
+      <c r="G7" s="22">
+        <v>9</v>
+      </c>
       <c r="H7" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="15">
@@ -803,22 +826,28 @@
         <v>11</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13"/>
+        <v>5</v>
+      </c>
+      <c r="C8" s="13">
+        <v>9</v>
+      </c>
       <c r="D8" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="14"/>
+        <v>0.45</v>
+      </c>
+      <c r="E8" s="22">
+        <v>9</v>
+      </c>
       <c r="F8" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="14"/>
+        <v>0.45</v>
+      </c>
+      <c r="G8" s="22">
+        <v>9</v>
+      </c>
       <c r="H8" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="15">
@@ -831,22 +860,28 @@
         <v>12</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="C9" s="13">
+        <v>7</v>
+      </c>
       <c r="D9" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="14"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="E9" s="22">
+        <v>7</v>
+      </c>
       <c r="F9" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="14"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="G9" s="22">
+        <v>7</v>
+      </c>
       <c r="H9" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="15">
@@ -859,22 +894,28 @@
         <v>13</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="13">
+        <v>9</v>
+      </c>
       <c r="D10" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="14"/>
+        <v>0.9</v>
+      </c>
+      <c r="E10" s="22">
+        <v>5</v>
+      </c>
       <c r="F10" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="22">
+        <v>5</v>
+      </c>
       <c r="H10" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="15">
@@ -887,22 +928,28 @@
         <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="16"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="16">
+        <v>5</v>
+      </c>
       <c r="D11" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="17"/>
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="17">
+        <v>7</v>
+      </c>
       <c r="F11" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="17"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="G11" s="17">
+        <v>7</v>
+      </c>
       <c r="H11" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="19">
@@ -918,17 +965,17 @@
       <c r="C12" s="16"/>
       <c r="D12" s="17">
         <f>SUM(D4:D11)</f>
-        <v>0</v>
+        <v>5.3500000000000005</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="18">
         <f>SUM(F4:F11)</f>
-        <v>0</v>
+        <v>7.0500000000000007</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18">
         <f>SUM(H4:H11)</f>
-        <v>0</v>
+        <v>7.3000000000000007</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="18">

</xml_diff>